<commit_message>
Adding 'Violence USE FOR Attempted murder'
</commit_message>
<xml_diff>
--- a/CTI.xlsx
+++ b/CTI.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\My Documents\Subject Headings\Children's Theme Index\GitHub\CTI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{925D92B1-3C19-47AF-A547-CA487FE8F5B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E735DFF2-CB5D-47E7-B91D-4925031A3320}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{EFCC635C-F9A6-442E-B628-876A5964CC75}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{EFCC635C-F9A6-442E-B628-876A5964CC75}"/>
   </bookViews>
   <sheets>
     <sheet name="Topical" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4709" uniqueCount="3048">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4710" uniqueCount="3049">
   <si>
     <t>USE FOR</t>
   </si>
@@ -9174,6 +9174,9 @@
   </si>
   <si>
     <t>CTIform00028</t>
+  </si>
+  <si>
+    <t>Attempted murder</t>
   </si>
 </sst>
 </file>
@@ -9562,9 +9565,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{729BB61C-91EA-4AAA-AF5F-904D4BA3CE5F}">
   <dimension ref="A1:G1377"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A193" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A210" sqref="A210"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A1143" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D1170" sqref="D1170"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23918,6 +23921,9 @@
       </c>
       <c r="C1169" t="s">
         <v>1287</v>
+      </c>
+      <c r="D1169" t="s">
+        <v>3048</v>
       </c>
       <c r="E1169" t="s">
         <v>1629</v>
@@ -26322,7 +26328,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65E92F3D-6A46-4853-BF96-D7DA551906FD}">
   <dimension ref="A1:G1382"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
@@ -27022,6 +27028,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <SharedWithUsers xmlns="6fffc368-2bf1-4b0d-b1b9-70dd7dd20a26">
@@ -27045,15 +27060,6 @@
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4AB86D2E-9309-4157-94EC-87BC40F81B9E}">
   <ds:schemaRefs>
@@ -27074,6 +27080,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DCF79B14-FC28-41CB-993F-0E5FAE3CA977}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4F8F3A3B-7903-49F7-9813-DD46116F01C3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -27081,12 +27095,4 @@
     <ds:schemaRef ds:uri="6fffc368-2bf1-4b0d-b1b9-70dd7dd20a26"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DCF79B14-FC28-41CB-993F-0E5FAE3CA977}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>